<commit_message>
add detail design teamplate
</commit_message>
<xml_diff>
--- a/ReadyToWork_BasicDesign.xlsx
+++ b/ReadyToWork_BasicDesign.xlsx
@@ -12,8 +12,9 @@
     <sheet name="Function List" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Task" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Database" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Q&amp;A" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Architechture design" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Detail Design_sample" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Q&amp;A" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Architechture design" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t xml:space="preserve">Todo-list-app là ứng dụng cho phép quản lý danh sách công việc cần làm.</t>
   </si>
@@ -159,6 +160,138 @@
   </si>
   <si>
     <t xml:space="preserve">Đặt Q&amp;A cho từng task ở sheet Function List (Xem ví dụ Q&amp;A về Login ở guideline)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chỉ một sơ đồ ERP cho toàn bộ ứng dunjg, được định  nghĩa ở đây. Khi modifying, cần note  rõ ai làm, làm lúc nào, lý do nào modify?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lý do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm bảng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sơ đồ ERP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detail design sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mục đích: Hướng dẫn member làm detail design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quy tắc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detail design của mỗi một task(cột D) trong function list sẽ là 1 sheet trong file này</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kết hợp SRS(up to date) và function list =&gt; để làm detail design ở mức overview cần thể hiện được các thông tin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. flow logic: step by step của chức năng: có thể vẽ biểu đồ hoạt động hoặc note gạch đầu dòng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b. Xác định được đối tượng thao tác trong function. Detail xem ở sheet: Detail design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c. Xác định được các entity để xây dựng database ( chỉ 1 sơ đổ ERP cho tất cả, khi cần update thì nhớ ghi rõ lịch sử cập nhật)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ví dụ về task Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business flow: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open site &lt;hostname&gt;/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User điền thông tin đăng nhập gồm: username/password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client kiểm tra format dữ liệu user nhập vào</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trường hợp user name vượt quá 10 ký từ =&gt; thông báo lỗi vượt quá 10 ý tư… → end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trường hợp n…. → end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client gửi thông tin username/password lên server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client nhận thông tin từ server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trường hợp thành công → chuyển sang site home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trường hợp có lỗi, hiển thị lỗi → end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Các đối tượng thao tác</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người dùng: có hoặc không có tài khoản trong hệ thống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hệ thống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xác định entity/Class của hệ thống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thông tin người dùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message thông báo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yêu cầu từ phía client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestAPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phản hồi từ server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResponseAPI</t>
   </si>
   <si>
     <t xml:space="preserve">Q&amp;A Function</t>
@@ -229,9 +362,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tien_Huy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chanh</t>
   </si>
   <si>
     <t xml:space="preserve">15/01/2020</t>
@@ -453,26 +583,8 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Về logic hãy là như bạn đề xuất.
-Về thông tin form, hãy follow theo các thông tin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: Tiêu đề, nội dung, trạng thái, người thực thiện, thời gian thực hiện</t>
-    </r>
+    <t xml:space="preserve">Về logic hãy là như bạn đề xuất.
+Về thông tin form, hãy follow theo các thông tin: Tiêu đề, nội dung, trạng thái, người thực thiện, thời gian thực hiện</t>
   </si>
   <si>
     <r>
@@ -701,6 +813,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -722,12 +841,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -791,7 +904,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -808,6 +921,26 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -816,15 +949,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -846,10 +975,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -918,7 +1043,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF4C4C4C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1040,7 +1165,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1233,17 +1358,89 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1259,249 +1456,447 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="2.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="80.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="42.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="4" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="11.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="4" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="6" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="2.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="80.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="42.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="9" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="9" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="9" style="9" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="9" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="B1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="190.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="190.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>56</v>
+      <c r="H2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="285" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="13" t="n">
+      <c r="C3" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>56</v>
+      <c r="H3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="13" t="n">
+      <c r="C4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>56</v>
+      <c r="H4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="285" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="13" t="n">
+      <c r="C5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H5" s="13" t="n">
+      <c r="H5" s="17" t="n">
         <v>44105</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>56</v>
+      <c r="I5" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="13" t="n">
+      <c r="C6" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>56</v>
+      <c r="H6" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="163.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="13" t="n">
+      <c r="C7" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>56</v>
+      <c r="H7" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="13" t="n">
+      <c r="C8" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="17" t="n">
         <v>44075</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>56</v>
+      <c r="H8" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1515,7 +1910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>